<commit_message>
add maintenance cycle api
</commit_message>
<xml_diff>
--- a/etc/rules/useful_life_rules.drl.xlsx
+++ b/etc/rules/useful_life_rules.drl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Quang Duong\Projects UIT\Thesis\hometopia\rule-service\src\main\resources\rule_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A912EA5-A2D5-4E99-9D6C-D7A0E6FB1A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF215DC6-6712-4D10-BD85-56E7DBE255A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Import</t>
   </si>
@@ -74,6 +74,84 @@
   </si>
   <si>
     <t>$assetUsefulLife.getCategory() in ($param)</t>
+  </si>
+  <si>
+    <t>AssetCategory.SOUND_SYSTEM</t>
+  </si>
+  <si>
+    <t>AssetCategory.PROJECTOR</t>
+  </si>
+  <si>
+    <t>AssetCategory.AIR_CONDITIONER</t>
+  </si>
+  <si>
+    <t>AssetCategory.LIGHTING</t>
+  </si>
+  <si>
+    <t>AssetCategory.AIR_PURIFIER</t>
+  </si>
+  <si>
+    <t>AssetCategory.STOVE</t>
+  </si>
+  <si>
+    <t>AssetCategory.MICROWAVE</t>
+  </si>
+  <si>
+    <t>AssetCategory.OVEN</t>
+  </si>
+  <si>
+    <t>AssetCategory.REFRIGERATOR</t>
+  </si>
+  <si>
+    <t>AssetCategory.WATER_PURIFIER</t>
+  </si>
+  <si>
+    <t>AssetCategory.RANGE_HOOD</t>
+  </si>
+  <si>
+    <t>AssetCategory.BED</t>
+  </si>
+  <si>
+    <t>AssetCategory.CAR</t>
+  </si>
+  <si>
+    <t>AssetCategory.WARDROBE</t>
+  </si>
+  <si>
+    <t>AssetCategory.FAN</t>
+  </si>
+  <si>
+    <t>AssetCategory.LAMP</t>
+  </si>
+  <si>
+    <t>AssetCategory.SHOWER</t>
+  </si>
+  <si>
+    <t>AssetCategory.BATHTUB</t>
+  </si>
+  <si>
+    <t>AssetCategory.SINK</t>
+  </si>
+  <si>
+    <t>AssetCategory.WATER_HEATER</t>
+  </si>
+  <si>
+    <t>AssetCategory.EXHAUST_FAN</t>
+  </si>
+  <si>
+    <t>AssetCategory.WASHING_MACHINE</t>
+  </si>
+  <si>
+    <t>AssetCategory.DRYER</t>
+  </si>
+  <si>
+    <t>AssetCategory.CLOTHES_RACK</t>
+  </si>
+  <si>
+    <t>AssetCategory.IRON</t>
+  </si>
+  <si>
+    <t>AssetCategory.CHAIR</t>
   </si>
 </sst>
 </file>
@@ -398,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,23 +557,231 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1">
-        <v>7</v>
+      <c r="C9">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
         <v>12</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C37">
         <v>4</v>
       </c>
     </row>

</xml_diff>